<commit_message>
new kest data/parsed some xlsx to csv/vwc analysis
</commit_message>
<xml_diff>
--- a/data/Experiment/Pre/InitialVWC.xlsx
+++ b/data/Experiment/Pre/InitialVWC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Pre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DEE804-786A-F149-A176-CE95E8C0075D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EADB2D8-F186-0D47-B55B-450148968172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17120" activeTab="3" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17400" windowHeight="17180" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIPO" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,8 @@
     <definedName name="_xlchart.v1.5" hidden="1">PIFL!$B$2:$B$61</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">PIEN!$B$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">PIEN!$B$2:$B$61</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">PIEN!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">PIEN!$B$2:$B$61</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="243">
   <si>
     <t>PIPO1</t>
   </si>
@@ -777,6 +775,9 @@
   </si>
   <si>
     <t>VWC_1000</t>
+  </si>
+  <si>
+    <t>VWC_perc</t>
   </si>
 </sst>
 </file>
@@ -3268,8 +3269,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3505200" y="6619240"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="3512820" y="6619240"/>
+              <a:ext cx="4584700" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3351,8 +3352,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7701446" y="3949976"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7676598" y="3876537"/>
+              <a:ext cx="4558196" cy="2692952"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3434,8 +3435,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6049818" y="7593445"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="6009409" y="7427190"/>
+              <a:ext cx="4543136" cy="2683164"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3517,8 +3518,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3505200" y="6822440"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="3515360" y="6822440"/>
+              <a:ext cx="4584700" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3868,10 +3869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F958DE17-0E59-E849-A835-10176DABDFD5}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="125" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3879,492 +3880,735 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>B2/10</f>
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" ref="C3:C61" si="0">B3/10</f>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>124</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>128</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>102</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16">
         <v>132</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>122</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>127</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>125</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>131</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>126</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>132</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>127</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>139</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B28">
         <v>122</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B29">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <v>118</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <v>107</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34">
         <v>113</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37">
         <v>121</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38">
         <v>125</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <v>130</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>133</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>121</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42">
         <v>122</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>128</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>121</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45">
         <v>121</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46">
         <v>127</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48">
         <v>131</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49">
         <v>144</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>91</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B52">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>138</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B54">
         <v>121</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B55">
         <v>134</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56">
         <v>94</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B57">
         <v>133</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B58">
         <v>137</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B59">
         <v>125</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B60">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B61">
         <v>121</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
       </c>
     </row>
   </sheetData>
@@ -4376,500 +4620,743 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E06963-B773-F348-8854-A3523910E721}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="92" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B2">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>B2/10</f>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B3">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" ref="C3:C61" si="0">B3/10</f>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B4">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B5">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B6">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B7">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B8">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B9">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B10">
         <v>154</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B11">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B12">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B13">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B14">
         <v>129</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B15">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B16">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B17">
         <v>139</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B18">
         <v>134</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B19">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B20">
         <v>139</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B21">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B22">
         <v>130</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B23">
         <v>135</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B24">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B25">
         <v>132</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B26">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B27">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B28">
         <v>110</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B29">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B30">
         <v>120</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B31">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B32">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B33">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B34">
         <v>136</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B35">
         <v>136</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B36">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B37">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B38">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B39">
         <v>123</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B40">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B41">
         <v>110</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B42">
         <v>125</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B43">
         <v>135</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B44">
         <v>117</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B45">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B46">
         <v>149</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B47">
         <v>138</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B48">
         <v>91</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B49">
         <v>120</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B50">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B51">
         <v>131</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B52">
         <v>116</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B53">
         <v>115</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B54">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B55">
         <v>122</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B56">
         <v>117</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B57">
         <v>114</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B58">
         <v>136</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B59">
         <v>128</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B60">
         <v>129</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B61">
         <v>123</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>12.3</v>
       </c>
     </row>
   </sheetData>
@@ -4880,500 +5367,743 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B18CAA-D5E2-8F4D-8617-88F8364D5DB9}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B2">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>B2/10</f>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B3">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" ref="C3:C61" si="0">B3/10</f>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B4">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B5">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B6">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B7">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B8">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B9">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B10">
         <v>129</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B11">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B12">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B13">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B14">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B15">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B16">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B18">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B20">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B21">
         <v>103</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B22">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B23">
         <v>117</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B24">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B25">
         <v>144</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B26">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B27">
         <v>117</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B28">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B29">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B30">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B31">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B32">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B33">
         <v>125</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B34">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B35">
         <v>127</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B36">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B37">
         <v>127</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B38">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B39">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B40">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B41">
         <v>132</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B42">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B43">
         <v>115</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B44">
         <v>121</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B45">
         <v>115</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B46">
         <v>124</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B47">
         <v>109</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B48">
         <v>113</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B49">
         <v>134</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B50">
         <v>127</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B51">
         <v>108</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B52">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B53">
         <v>130</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B54">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B55">
         <v>126</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B56">
         <v>119</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B57">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B58">
         <v>127</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B59">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B60">
         <v>114</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B61">
         <v>109</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>10.9</v>
       </c>
     </row>
   </sheetData>
@@ -5384,500 +6114,743 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115E6809-C6E9-4B42-AF0B-D16D811C3B7F}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B2">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>B2/10</f>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B3">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" ref="C3:C61" si="0">B3/10</f>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B4">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B5">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B6">
         <v>149</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>186</v>
       </c>
       <c r="B7">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B8">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B9">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B10">
         <v>124</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B11">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B12">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B13">
         <v>133</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B14">
         <v>147</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B15">
         <v>135</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B16">
         <v>134</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B17">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B18">
         <v>185</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>198</v>
       </c>
       <c r="B19">
         <v>128</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B20">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B21">
         <v>134</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B22">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B23">
         <v>138</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B24">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B25">
         <v>128</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>205</v>
       </c>
       <c r="B26">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B27">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B28">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B29">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B30">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B31">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B32">
         <v>131</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B33">
         <v>106</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B34">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B35">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B36">
         <v>129</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B37">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B38">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B39">
         <v>108</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B40">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B41">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B42">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B43">
         <v>115</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B44">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B45">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B46">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B47">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B48">
         <v>110</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B49">
         <v>118</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B50">
         <v>106</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B51">
         <v>129</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B52">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B53">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B54">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B55">
         <v>127</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B56">
         <v>103</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>236</v>
       </c>
       <c r="B57">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B58">
         <v>108</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B59">
         <v>111</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>239</v>
       </c>
       <c r="B60">
         <v>129</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B61">
         <v>121</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>12.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>